<commit_message>
Test case 1 to 6
</commit_message>
<xml_diff>
--- a/cypress/fixtures/excelData.xlsx
+++ b/cypress/fixtures/excelData.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Projects\Savvas\cypress\fixtures\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="8510"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
   </si>
+  <si>
+    <t>MSuite49win10chrome_teacher04</t>
+  </si>
+  <si>
+    <t>testing123$</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,42 +83,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -127,10 +130,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -168,71 +171,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -260,7 +263,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -283,11 +286,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -296,13 +299,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -312,7 +315,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -321,7 +324,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -330,7 +333,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,10 +341,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -412,36 +415,34 @@
   </sheetPr>
   <dimension ref="A1:U191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="8.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="16.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,9 +469,13 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -491,7 +496,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -514,7 +519,7 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -537,7 +542,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -560,7 +565,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -583,7 +588,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -606,7 +611,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -629,7 +634,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -652,7 +657,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -675,7 +680,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -698,7 +703,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -721,7 +726,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -744,7 +749,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -767,7 +772,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -790,7 +795,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -813,7 +818,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -836,7 +841,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -859,7 +864,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -882,7 +887,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -905,7 +910,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -928,7 +933,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -951,7 +956,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -974,7 +979,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -997,7 +1002,7 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1020,7 +1025,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1043,7 +1048,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1066,7 +1071,7 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1089,7 +1094,7 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
     </row>
-    <row r="29" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1112,7 +1117,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1135,7 +1140,7 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1158,7 +1163,7 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1181,7 +1186,7 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
     </row>
-    <row r="33" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1204,7 +1209,7 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
     </row>
-    <row r="34" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1227,7 +1232,7 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
     </row>
-    <row r="35" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1250,7 +1255,7 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1273,7 +1278,7 @@
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
     </row>
-    <row r="37" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1296,7 +1301,7 @@
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1319,7 +1324,7 @@
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
     </row>
-    <row r="39" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1342,7 +1347,7 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
     </row>
-    <row r="40" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1365,7 +1370,7 @@
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
     </row>
-    <row r="41" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1388,7 +1393,7 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
     </row>
-    <row r="42" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1411,7 +1416,7 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
     </row>
-    <row r="43" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1434,7 +1439,7 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
     </row>
-    <row r="44" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1457,7 +1462,7 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
     </row>
-    <row r="45" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1480,7 +1485,7 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
     </row>
-    <row r="46" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1503,7 +1508,7 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
     </row>
-    <row r="47" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1526,7 +1531,7 @@
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
     </row>
-    <row r="48" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1549,7 +1554,7 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
     </row>
-    <row r="49" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1572,7 +1577,7 @@
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
     </row>
-    <row r="50" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1595,7 +1600,7 @@
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
     </row>
-    <row r="51" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1618,7 +1623,7 @@
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
     </row>
-    <row r="52" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1641,7 +1646,7 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
     </row>
-    <row r="53" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1664,7 +1669,7 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
     </row>
-    <row r="54" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1687,7 +1692,7 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
     </row>
-    <row r="55" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1710,7 +1715,7 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
     </row>
-    <row r="56" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1733,7 +1738,7 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
     </row>
-    <row r="57" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1756,7 +1761,7 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
     </row>
-    <row r="58" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1779,7 +1784,7 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
     </row>
-    <row r="59" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1802,7 +1807,7 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
     </row>
-    <row r="60" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1825,7 +1830,7 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
     </row>
-    <row r="61" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1848,7 +1853,7 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
     </row>
-    <row r="62" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1871,7 +1876,7 @@
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
     </row>
-    <row r="63" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1894,7 +1899,7 @@
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
     </row>
-    <row r="64" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1917,7 +1922,7 @@
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
     </row>
-    <row r="65" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1940,7 +1945,7 @@
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
     </row>
-    <row r="66" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1963,7 +1968,7 @@
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
     </row>
-    <row r="67" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1986,7 +1991,7 @@
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
     </row>
-    <row r="68" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2009,7 +2014,7 @@
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
     </row>
-    <row r="69" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2032,7 +2037,7 @@
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
     </row>
-    <row r="70" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2055,7 +2060,7 @@
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
     </row>
-    <row r="71" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2078,7 +2083,7 @@
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
     </row>
-    <row r="72" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2101,7 +2106,7 @@
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
     </row>
-    <row r="73" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2124,7 +2129,7 @@
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
     </row>
-    <row r="74" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2147,7 +2152,7 @@
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
     </row>
-    <row r="75" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2170,7 +2175,7 @@
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
     </row>
-    <row r="76" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2193,7 +2198,7 @@
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
     </row>
-    <row r="77" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2216,7 +2221,7 @@
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
     </row>
-    <row r="78" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2239,7 +2244,7 @@
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
     </row>
-    <row r="79" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2262,7 +2267,7 @@
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
     </row>
-    <row r="80" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2285,7 +2290,7 @@
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
     </row>
-    <row r="81" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2308,7 +2313,7 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
     </row>
-    <row r="82" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2331,7 +2336,7 @@
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
     </row>
-    <row r="83" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2354,7 +2359,7 @@
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
     </row>
-    <row r="84" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2377,7 +2382,7 @@
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
     </row>
-    <row r="85" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2400,7 +2405,7 @@
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
     </row>
-    <row r="86" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2423,7 +2428,7 @@
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
     </row>
-    <row r="87" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2446,7 +2451,7 @@
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
     </row>
-    <row r="88" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2469,7 +2474,7 @@
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
     </row>
-    <row r="89" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2492,7 +2497,7 @@
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
     </row>
-    <row r="90" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2515,7 +2520,7 @@
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
     </row>
-    <row r="91" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2538,7 +2543,7 @@
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
     </row>
-    <row r="92" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2561,7 +2566,7 @@
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
     </row>
-    <row r="93" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2584,7 +2589,7 @@
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
     </row>
-    <row r="94" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2607,7 +2612,7 @@
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
     </row>
-    <row r="95" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2630,7 +2635,7 @@
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
     </row>
-    <row r="96" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2653,7 +2658,7 @@
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
     </row>
-    <row r="97" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2676,7 +2681,7 @@
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
     </row>
-    <row r="98" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2699,7 +2704,7 @@
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
     </row>
-    <row r="99" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2722,7 +2727,7 @@
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
     </row>
-    <row r="100" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2745,7 +2750,7 @@
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
     </row>
-    <row r="101" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2768,7 +2773,7 @@
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
     </row>
-    <row r="102" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2791,7 +2796,7 @@
       <c r="T102" s="1"/>
       <c r="U102" s="1"/>
     </row>
-    <row r="103" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2814,7 +2819,7 @@
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
     </row>
-    <row r="104" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2837,7 +2842,7 @@
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
     </row>
-    <row r="105" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2860,7 +2865,7 @@
       <c r="T105" s="1"/>
       <c r="U105" s="1"/>
     </row>
-    <row r="106" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2883,7 +2888,7 @@
       <c r="T106" s="1"/>
       <c r="U106" s="1"/>
     </row>
-    <row r="107" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2906,7 +2911,7 @@
       <c r="T107" s="1"/>
       <c r="U107" s="1"/>
     </row>
-    <row r="108" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2929,7 +2934,7 @@
       <c r="T108" s="1"/>
       <c r="U108" s="1"/>
     </row>
-    <row r="109" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2952,7 +2957,7 @@
       <c r="T109" s="1"/>
       <c r="U109" s="1"/>
     </row>
-    <row r="110" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2975,7 +2980,7 @@
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
     </row>
-    <row r="111" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2998,7 +3003,7 @@
       <c r="T111" s="1"/>
       <c r="U111" s="1"/>
     </row>
-    <row r="112" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3021,7 +3026,7 @@
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
     </row>
-    <row r="113" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3044,7 +3049,7 @@
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
     </row>
-    <row r="114" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3067,7 +3072,7 @@
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
     </row>
-    <row r="115" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3090,7 +3095,7 @@
       <c r="T115" s="1"/>
       <c r="U115" s="1"/>
     </row>
-    <row r="116" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3113,7 +3118,7 @@
       <c r="T116" s="1"/>
       <c r="U116" s="1"/>
     </row>
-    <row r="117" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3136,7 +3141,7 @@
       <c r="T117" s="1"/>
       <c r="U117" s="1"/>
     </row>
-    <row r="118" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3159,7 +3164,7 @@
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
     </row>
-    <row r="119" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3182,7 +3187,7 @@
       <c r="T119" s="1"/>
       <c r="U119" s="1"/>
     </row>
-    <row r="120" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3205,7 +3210,7 @@
       <c r="T120" s="1"/>
       <c r="U120" s="1"/>
     </row>
-    <row r="121" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3228,7 +3233,7 @@
       <c r="T121" s="1"/>
       <c r="U121" s="1"/>
     </row>
-    <row r="122" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3251,7 +3256,7 @@
       <c r="T122" s="1"/>
       <c r="U122" s="1"/>
     </row>
-    <row r="123" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3274,7 +3279,7 @@
       <c r="T123" s="1"/>
       <c r="U123" s="1"/>
     </row>
-    <row r="124" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3297,7 +3302,7 @@
       <c r="T124" s="1"/>
       <c r="U124" s="1"/>
     </row>
-    <row r="125" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3320,7 +3325,7 @@
       <c r="T125" s="1"/>
       <c r="U125" s="1"/>
     </row>
-    <row r="126" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3343,7 +3348,7 @@
       <c r="T126" s="1"/>
       <c r="U126" s="1"/>
     </row>
-    <row r="127" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3366,7 +3371,7 @@
       <c r="T127" s="1"/>
       <c r="U127" s="1"/>
     </row>
-    <row r="128" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3389,7 +3394,7 @@
       <c r="T128" s="1"/>
       <c r="U128" s="1"/>
     </row>
-    <row r="129" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3412,7 +3417,7 @@
       <c r="T129" s="1"/>
       <c r="U129" s="1"/>
     </row>
-    <row r="130" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3435,7 +3440,7 @@
       <c r="T130" s="1"/>
       <c r="U130" s="1"/>
     </row>
-    <row r="131" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3458,7 +3463,7 @@
       <c r="T131" s="1"/>
       <c r="U131" s="1"/>
     </row>
-    <row r="132" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3481,7 +3486,7 @@
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
     </row>
-    <row r="133" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3504,7 +3509,7 @@
       <c r="T133" s="1"/>
       <c r="U133" s="1"/>
     </row>
-    <row r="134" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3527,7 +3532,7 @@
       <c r="T134" s="1"/>
       <c r="U134" s="1"/>
     </row>
-    <row r="135" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3550,7 +3555,7 @@
       <c r="T135" s="1"/>
       <c r="U135" s="1"/>
     </row>
-    <row r="136" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3573,7 +3578,7 @@
       <c r="T136" s="1"/>
       <c r="U136" s="1"/>
     </row>
-    <row r="137" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3596,7 +3601,7 @@
       <c r="T137" s="1"/>
       <c r="U137" s="1"/>
     </row>
-    <row r="138" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3619,7 +3624,7 @@
       <c r="T138" s="1"/>
       <c r="U138" s="1"/>
     </row>
-    <row r="139" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3642,7 +3647,7 @@
       <c r="T139" s="1"/>
       <c r="U139" s="1"/>
     </row>
-    <row r="140" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3665,7 +3670,7 @@
       <c r="T140" s="1"/>
       <c r="U140" s="1"/>
     </row>
-    <row r="141" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3688,7 +3693,7 @@
       <c r="T141" s="1"/>
       <c r="U141" s="1"/>
     </row>
-    <row r="142" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3711,7 +3716,7 @@
       <c r="T142" s="1"/>
       <c r="U142" s="1"/>
     </row>
-    <row r="143" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3734,7 +3739,7 @@
       <c r="T143" s="1"/>
       <c r="U143" s="1"/>
     </row>
-    <row r="144" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3757,7 +3762,7 @@
       <c r="T144" s="1"/>
       <c r="U144" s="1"/>
     </row>
-    <row r="145" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3780,7 +3785,7 @@
       <c r="T145" s="1"/>
       <c r="U145" s="1"/>
     </row>
-    <row r="146" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3803,7 +3808,7 @@
       <c r="T146" s="1"/>
       <c r="U146" s="1"/>
     </row>
-    <row r="147" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3826,7 +3831,7 @@
       <c r="T147" s="1"/>
       <c r="U147" s="1"/>
     </row>
-    <row r="148" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3849,7 +3854,7 @@
       <c r="T148" s="1"/>
       <c r="U148" s="1"/>
     </row>
-    <row r="149" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3872,7 +3877,7 @@
       <c r="T149" s="1"/>
       <c r="U149" s="1"/>
     </row>
-    <row r="150" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3895,7 +3900,7 @@
       <c r="T150" s="1"/>
       <c r="U150" s="1"/>
     </row>
-    <row r="151" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3918,7 +3923,7 @@
       <c r="T151" s="1"/>
       <c r="U151" s="1"/>
     </row>
-    <row r="152" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3941,7 +3946,7 @@
       <c r="T152" s="1"/>
       <c r="U152" s="1"/>
     </row>
-    <row r="153" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3964,7 +3969,7 @@
       <c r="T153" s="1"/>
       <c r="U153" s="1"/>
     </row>
-    <row r="154" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3987,7 +3992,7 @@
       <c r="T154" s="1"/>
       <c r="U154" s="1"/>
     </row>
-    <row r="155" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4010,7 +4015,7 @@
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
     </row>
-    <row r="156" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4033,7 +4038,7 @@
       <c r="T156" s="1"/>
       <c r="U156" s="1"/>
     </row>
-    <row r="157" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4056,7 +4061,7 @@
       <c r="T157" s="1"/>
       <c r="U157" s="1"/>
     </row>
-    <row r="158" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4079,7 +4084,7 @@
       <c r="T158" s="1"/>
       <c r="U158" s="1"/>
     </row>
-    <row r="159" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4102,7 +4107,7 @@
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
     </row>
-    <row r="160" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4125,7 +4130,7 @@
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
     </row>
-    <row r="161" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4148,7 +4153,7 @@
       <c r="T161" s="1"/>
       <c r="U161" s="1"/>
     </row>
-    <row r="162" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4171,7 +4176,7 @@
       <c r="T162" s="1"/>
       <c r="U162" s="1"/>
     </row>
-    <row r="163" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4194,7 +4199,7 @@
       <c r="T163" s="1"/>
       <c r="U163" s="1"/>
     </row>
-    <row r="164" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4217,7 +4222,7 @@
       <c r="T164" s="1"/>
       <c r="U164" s="1"/>
     </row>
-    <row r="165" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4240,7 +4245,7 @@
       <c r="T165" s="1"/>
       <c r="U165" s="1"/>
     </row>
-    <row r="166" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4263,7 +4268,7 @@
       <c r="T166" s="1"/>
       <c r="U166" s="1"/>
     </row>
-    <row r="167" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4286,7 +4291,7 @@
       <c r="T167" s="1"/>
       <c r="U167" s="1"/>
     </row>
-    <row r="168" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4309,7 +4314,7 @@
       <c r="T168" s="1"/>
       <c r="U168" s="1"/>
     </row>
-    <row r="169" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4332,7 +4337,7 @@
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
     </row>
-    <row r="170" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4355,7 +4360,7 @@
       <c r="T170" s="1"/>
       <c r="U170" s="1"/>
     </row>
-    <row r="171" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4378,7 +4383,7 @@
       <c r="T171" s="1"/>
       <c r="U171" s="1"/>
     </row>
-    <row r="172" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4401,7 +4406,7 @@
       <c r="T172" s="1"/>
       <c r="U172" s="1"/>
     </row>
-    <row r="173" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4424,7 +4429,7 @@
       <c r="T173" s="1"/>
       <c r="U173" s="1"/>
     </row>
-    <row r="174" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4447,7 +4452,7 @@
       <c r="T174" s="1"/>
       <c r="U174" s="1"/>
     </row>
-    <row r="175" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4470,7 +4475,7 @@
       <c r="T175" s="1"/>
       <c r="U175" s="1"/>
     </row>
-    <row r="176" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4493,7 +4498,7 @@
       <c r="T176" s="1"/>
       <c r="U176" s="1"/>
     </row>
-    <row r="177" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4516,7 +4521,7 @@
       <c r="T177" s="1"/>
       <c r="U177" s="1"/>
     </row>
-    <row r="178" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4539,7 +4544,7 @@
       <c r="T178" s="1"/>
       <c r="U178" s="1"/>
     </row>
-    <row r="179" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4562,7 +4567,7 @@
       <c r="T179" s="1"/>
       <c r="U179" s="1"/>
     </row>
-    <row r="180" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4585,7 +4590,7 @@
       <c r="T180" s="1"/>
       <c r="U180" s="1"/>
     </row>
-    <row r="181" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4608,7 +4613,7 @@
       <c r="T181" s="1"/>
       <c r="U181" s="1"/>
     </row>
-    <row r="182" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4631,7 +4636,7 @@
       <c r="T182" s="1"/>
       <c r="U182" s="1"/>
     </row>
-    <row r="183" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4654,7 +4659,7 @@
       <c r="T183" s="1"/>
       <c r="U183" s="1"/>
     </row>
-    <row r="184" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4677,7 +4682,7 @@
       <c r="T184" s="1"/>
       <c r="U184" s="1"/>
     </row>
-    <row r="185" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4700,7 +4705,7 @@
       <c r="T185" s="1"/>
       <c r="U185" s="1"/>
     </row>
-    <row r="186" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4723,7 +4728,7 @@
       <c r="T186" s="1"/>
       <c r="U186" s="1"/>
     </row>
-    <row r="187" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4746,7 +4751,7 @@
       <c r="T187" s="1"/>
       <c r="U187" s="1"/>
     </row>
-    <row r="188" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4769,7 +4774,7 @@
       <c r="T188" s="1"/>
       <c r="U188" s="1"/>
     </row>
-    <row r="189" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4792,7 +4797,7 @@
       <c r="T189" s="1"/>
       <c r="U189" s="1"/>
     </row>
-    <row r="190" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4815,7 +4820,7 @@
       <c r="T190" s="1"/>
       <c r="U190" s="1"/>
     </row>
-    <row r="191" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>

</xml_diff>